<commit_message>
add key test data
</commit_message>
<xml_diff>
--- a/excel/TestData.xlsx
+++ b/excel/TestData.xlsx
@@ -8,23 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geukg\OneDrive\문서\TSomSomm\lunaria-project\lunaria-data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50830CCB-2F16-4009-AD3F-88BD1766A87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897C6FF8-842C-4F90-A70E-6AEE31918C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5250" yWindow="1815" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TestData" sheetId="1" r:id="rId1"/>
-    <sheet name="MapData" sheetId="2" r:id="rId2"/>
+    <sheet name="KeyTestData" sheetId="3" r:id="rId1"/>
+    <sheet name="TestData" sheetId="1" r:id="rId2"/>
+    <sheet name="MapData" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
-  <si>
-    <t>int</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>string</t>
   </si>
@@ -76,6 +74,14 @@
   </si>
   <si>
     <t>Yellow</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>int;key</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -207,7 +213,7 @@
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -422,86 +428,86 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D819504-98C5-4DFA-B58D-891D00EC2C77}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5">
         <v>100</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="7">
         <v>80</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="8">
         <v>60</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -509,16 +515,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>160</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F10" s="10"/>
     </row>
   </sheetData>
@@ -528,6 +534,112 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5">
+        <v>100</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="7">
+        <v>80</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="8">
+        <v>60</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>160</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F10" s="10"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -543,17 +655,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>